<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@c5a9be0791075a361e304f507f7b100438408ac4 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-observation-lab.xlsx
+++ b/StructureDefinition-us-core-observation-lab.xlsx
@@ -75,7 +75,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>null (mailto:ehaas@healthedatainc.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -417,7 +417,7 @@
 </t>
   </si>
   <si>
-    <t>When the resource version last changed</t>
+    <t>When the resource last changed</t>
   </si>
   <si>
     <t>When the resource last changed - e.g. when the version changed.</t>

</xml_diff>